<commit_message>
Repeated the analysis with new asthma IR removing other states
</commit_message>
<xml_diff>
--- a/Results/Burden_by_state.xlsx
+++ b/Results/Burden_by_state.xlsx
@@ -287,10 +287,10 @@
         <v>7.3690271E7</v>
       </c>
       <c r="B2" t="n">
-        <v>751100.0</v>
+        <v>751300.0</v>
       </c>
       <c r="C2" t="n">
-        <v>132620.0</v>
+        <v>132640.0</v>
       </c>
       <c r="D2" t="n">
         <v>17.7</v>
@@ -480,7 +480,7 @@
         <v>2296157.0</v>
       </c>
       <c r="D9" t="n">
-        <v>23300.0</v>
+        <v>23400.0</v>
       </c>
       <c r="E9" t="n">
         <v>3070.0</v>
@@ -620,10 +620,10 @@
         <v>1.5577423E7</v>
       </c>
       <c r="D16" t="n">
-        <v>155900.0</v>
+        <v>156000.0</v>
       </c>
       <c r="E16" t="n">
-        <v>29540.0</v>
+        <v>29550.0</v>
       </c>
       <c r="F16" t="n">
         <v>18.9</v>
@@ -2690,7 +2690,7 @@
         <v>349385.0</v>
       </c>
       <c r="E87" t="n">
-        <v>3600.0</v>
+        <v>3700.0</v>
       </c>
       <c r="F87" t="n">
         <v>860.0</v>
@@ -8408,7 +8408,7 @@
         <v>5700.0</v>
       </c>
       <c r="F336" t="n">
-        <v>880.0</v>
+        <v>890.0</v>
       </c>
       <c r="G336" t="n">
         <v>15.5</v>
@@ -12957,7 +12957,7 @@
         <v>310926.0</v>
       </c>
       <c r="E534" t="n">
-        <v>3200.0</v>
+        <v>3300.0</v>
       </c>
       <c r="F534" t="n">
         <v>500.0</v>
@@ -21725,7 +21725,7 @@
         <v>349385.0</v>
       </c>
       <c r="E89" t="n">
-        <v>3600.0</v>
+        <v>3700.0</v>
       </c>
       <c r="F89" t="n">
         <v>860.0</v>
@@ -27420,7 +27420,7 @@
         <v>5700.0</v>
       </c>
       <c r="F337" t="n">
-        <v>880.0</v>
+        <v>890.0</v>
       </c>
       <c r="G337" t="n">
         <v>15.5</v>
@@ -32084,7 +32084,7 @@
         <v>310926.0</v>
       </c>
       <c r="E540" t="n">
-        <v>3200.0</v>
+        <v>3300.0</v>
       </c>
       <c r="F540" t="n">
         <v>500.0</v>
@@ -39232,7 +39232,7 @@
         <v>2281635.0</v>
       </c>
       <c r="C33" t="n">
-        <v>23800.0</v>
+        <v>23900.0</v>
       </c>
       <c r="D33" t="n">
         <v>3080.0</v>
@@ -39388,7 +39388,7 @@
         <v>15600.0</v>
       </c>
       <c r="D42" t="n">
-        <v>2420.0</v>
+        <v>2430.0</v>
       </c>
       <c r="E42" t="n">
         <v>15.5</v>
@@ -39602,10 +39602,10 @@
         <v>5.2932624E7</v>
       </c>
       <c r="C4" t="n">
-        <v>538900.0</v>
+        <v>539000.0</v>
       </c>
       <c r="D4" t="n">
-        <v>109490.0</v>
+        <v>109510.0</v>
       </c>
       <c r="E4" t="n">
         <v>20.3</v>
@@ -39669,7 +39669,7 @@
         <v>133200.0</v>
       </c>
       <c r="D3" t="n">
-        <v>24800.0</v>
+        <v>24810.0</v>
       </c>
       <c r="E3" t="n">
         <v>18.6</v>
@@ -39700,10 +39700,10 @@
         <v>2.1953876E7</v>
       </c>
       <c r="C5" t="n">
-        <v>222700.0</v>
+        <v>222800.0</v>
       </c>
       <c r="D5" t="n">
-        <v>37590.0</v>
+        <v>37600.0</v>
       </c>
       <c r="E5" t="n">
         <v>16.9</v>
@@ -40070,7 +40070,7 @@
         <v>10000.0</v>
       </c>
       <c r="E16" t="n">
-        <v>2640.0</v>
+        <v>2650.0</v>
       </c>
       <c r="F16" t="n">
         <v>26.4</v>
@@ -40267,10 +40267,10 @@
         <v>3489032.0</v>
       </c>
       <c r="D26" t="n">
-        <v>36400.0</v>
+        <v>36500.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4940.0</v>
+        <v>4950.0</v>
       </c>
       <c r="F26" t="n">
         <v>13.6</v>
@@ -40927,7 +40927,7 @@
         <v>1277514.0</v>
       </c>
       <c r="D59" t="n">
-        <v>13300.0</v>
+        <v>13400.0</v>
       </c>
       <c r="E59" t="n">
         <v>2300.0</v>
@@ -41610,7 +41610,7 @@
         <v>7800.0</v>
       </c>
       <c r="E93" t="n">
-        <v>740.0</v>
+        <v>750.0</v>
       </c>
       <c r="F93" t="n">
         <v>9.6</v>
@@ -42190,7 +42190,7 @@
         <v>8700.0</v>
       </c>
       <c r="E122" t="n">
-        <v>1580.0</v>
+        <v>1590.0</v>
       </c>
       <c r="F122" t="n">
         <v>18.3</v>
@@ -43263,7 +43263,7 @@
         <v>3700.0</v>
       </c>
       <c r="E29" t="n">
-        <v>820.0</v>
+        <v>830.0</v>
       </c>
       <c r="F29" t="n">
         <v>22.1</v>
@@ -43740,7 +43740,7 @@
         <v>1259100.0</v>
       </c>
       <c r="D53" t="n">
-        <v>13100.0</v>
+        <v>13200.0</v>
       </c>
       <c r="E53" t="n">
         <v>1570.0</v>
@@ -47500,7 +47500,7 @@
         <v>378182.0</v>
       </c>
       <c r="D241" t="n">
-        <v>3900.0</v>
+        <v>4000.0</v>
       </c>
       <c r="E241" t="n">
         <v>640.0</v>
@@ -49176,7 +49176,7 @@
         <v>7800.0</v>
       </c>
       <c r="E32" t="n">
-        <v>740.0</v>
+        <v>750.0</v>
       </c>
       <c r="F32" t="n">
         <v>9.6</v>
@@ -50576,7 +50576,7 @@
         <v>10000.0</v>
       </c>
       <c r="E102" t="n">
-        <v>2640.0</v>
+        <v>2650.0</v>
       </c>
       <c r="F102" t="n">
         <v>26.4</v>
@@ -50653,10 +50653,10 @@
         <v>3489032.0</v>
       </c>
       <c r="D106" t="n">
-        <v>36400.0</v>
+        <v>36500.0</v>
       </c>
       <c r="E106" t="n">
-        <v>4940.0</v>
+        <v>4950.0</v>
       </c>
       <c r="F106" t="n">
         <v>13.6</v>
@@ -50873,7 +50873,7 @@
         <v>1277514.0</v>
       </c>
       <c r="D117" t="n">
-        <v>13300.0</v>
+        <v>13400.0</v>
       </c>
       <c r="E117" t="n">
         <v>2300.0</v>
@@ -51296,7 +51296,7 @@
         <v>8700.0</v>
       </c>
       <c r="E138" t="n">
-        <v>1580.0</v>
+        <v>1590.0</v>
       </c>
       <c r="F138" t="n">
         <v>18.3</v>
@@ -53286,7 +53286,7 @@
         <v>378182.0</v>
       </c>
       <c r="D91" t="n">
-        <v>3900.0</v>
+        <v>4000.0</v>
       </c>
       <c r="E91" t="n">
         <v>640.0</v>
@@ -54529,7 +54529,7 @@
         <v>3700.0</v>
       </c>
       <c r="E153" t="n">
-        <v>820.0</v>
+        <v>830.0</v>
       </c>
       <c r="F153" t="n">
         <v>22.1</v>
@@ -54606,7 +54606,7 @@
         <v>1259100.0</v>
       </c>
       <c r="D157" t="n">
-        <v>13100.0</v>
+        <v>13200.0</v>
       </c>
       <c r="E157" t="n">
         <v>1570.0</v>
@@ -57519,7 +57519,7 @@
         <v>2296157.0</v>
       </c>
       <c r="D10" t="n">
-        <v>23300.0</v>
+        <v>23400.0</v>
       </c>
       <c r="E10" t="n">
         <v>3070.0</v>
@@ -57679,10 +57679,10 @@
         <v>1.5577423E7</v>
       </c>
       <c r="D18" t="n">
-        <v>155900.0</v>
+        <v>156000.0</v>
       </c>
       <c r="E18" t="n">
-        <v>29540.0</v>
+        <v>29550.0</v>
       </c>
       <c r="F18" t="n">
         <v>18.9</v>

</xml_diff>